<commit_message>
Changes made to data/FantasyData.xlsx at Thu Aug  8 21:09:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/FantasyData.xlsx
+++ b/data/FantasyData.xlsx
@@ -32521,7 +32521,7 @@
     </row>
     <row r="911" spans="1:4">
       <c r="A911" t="s">
-        <v>554</v>
+        <v>396</v>
       </c>
       <c r="B911" t="s">
         <v>681</v>
@@ -32535,7 +32535,7 @@
     </row>
     <row r="912" spans="1:4">
       <c r="A912" t="s">
-        <v>396</v>
+        <v>554</v>
       </c>
       <c r="B912" t="s">
         <v>681</v>

</xml_diff>